<commit_message>
first new culture building
Theoretically, these buildings will give you levies BUT decrease
garrison size a bit, representing that you are taking people from the
holding and making them better fighters, but losing their ability to be
a part of the garrison.
</commit_message>
<xml_diff>
--- a/tsf4's Nightfort/cultural buildings checklist.xlsx
+++ b/tsf4's Nightfort/cultural buildings checklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Culture</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Iron Islander</t>
+  </si>
+  <si>
+    <t>1 of 8</t>
   </si>
 </sst>
 </file>
@@ -563,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -661,82 +664,85 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
family for bloody crescent & culture building work
</commit_message>
<xml_diff>
--- a/tsf4's Nightfort/cultural buildings checklist.xlsx
+++ b/tsf4's Nightfort/cultural buildings checklist.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t>Culture</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Pentoshi</t>
   </si>
   <si>
-    <t>Flatland Pentoshi</t>
-  </si>
-  <si>
     <t>Dornish</t>
   </si>
   <si>
@@ -247,15 +244,12 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Tribal only</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -576,11 +570,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -603,10 +597,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -615,7 +609,7 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -623,7 +617,7 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -641,10 +635,10 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -684,6 +678,9 @@
       <c r="A13" t="s">
         <v>15</v>
       </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
@@ -713,10 +710,10 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -738,6 +735,9 @@
       <c r="A22" t="s">
         <v>24</v>
       </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
@@ -784,7 +784,7 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -796,35 +796,38 @@
       <c r="A33" t="s">
         <v>35</v>
       </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>36</v>
       </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>37</v>
       </c>
-      <c r="B35" t="s">
-        <v>72</v>
+      <c r="E35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>38</v>
       </c>
-      <c r="E36">
-        <v>1</v>
+      <c r="C36" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>39</v>
       </c>
-      <c r="C37" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
@@ -840,6 +843,9 @@
       <c r="A40" t="s">
         <v>42</v>
       </c>
+      <c r="C40" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
@@ -850,21 +856,24 @@
       <c r="A42" t="s">
         <v>44</v>
       </c>
+      <c r="D42" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>45</v>
       </c>
-      <c r="D43" t="s">
-        <v>72</v>
+      <c r="B43" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>46</v>
       </c>
-      <c r="B44" t="s">
-        <v>72</v>
+      <c r="D44" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -891,14 +900,17 @@
       <c r="A49" t="s">
         <v>51</v>
       </c>
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>52</v>
       </c>
-      <c r="B50" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
@@ -924,19 +936,22 @@
       <c r="A55" t="s">
         <v>57</v>
       </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>58</v>
       </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>59</v>
       </c>
+      <c r="D57" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
@@ -947,14 +962,14 @@
       <c r="A59" t="s">
         <v>61</v>
       </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>62</v>
       </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
@@ -965,52 +980,47 @@
       <c r="A62" t="s">
         <v>64</v>
       </c>
+      <c r="C62" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>65</v>
       </c>
-      <c r="C63" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>67</v>
       </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C66" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>69</v>
       </c>
-      <c r="C67" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" t="s">
-        <v>71</v>
-      </c>
-      <c r="D69" t="s">
-        <v>72</v>
+      <c r="D68" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 more generic mercenaries added
Remembered the flags this time!
</commit_message>
<xml_diff>
--- a/tsf4's Nightfort/cultural buildings checklist.xlsx
+++ b/tsf4's Nightfort/cultural buildings checklist.xlsx
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -653,6 +653,9 @@
       <c r="A8" t="s">
         <v>10</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
@@ -943,6 +946,9 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>58</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
clearing out cultural buildings pending new idea & some edits to Hangman pirates
</commit_message>
<xml_diff>
--- a/tsf4's Nightfort/cultural buildings checklist.xlsx
+++ b/tsf4's Nightfort/cultural buildings checklist.xlsx
@@ -19,20 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Culture</t>
   </si>
   <si>
-    <t>Castle</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Temple</t>
-  </si>
-  <si>
     <t>Myrman</t>
   </si>
   <si>
@@ -234,16 +225,13 @@
     <t>Iron Islander</t>
   </si>
   <si>
-    <t>1 of 8</t>
-  </si>
-  <si>
     <t>Mercs</t>
   </si>
   <si>
     <t>Local</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>Level Completed</t>
   </si>
 </sst>
 </file>
@@ -571,483 +559,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="22.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="E7">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" t="s">
-        <v>71</v>
-      </c>
-      <c r="F33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="E55">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" t="s">
-        <v>58</v>
-      </c>
-      <c r="E56">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" t="s">
-        <v>61</v>
-      </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="C62" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" t="s">
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" t="s">
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" t="s">
-        <v>68</v>
-      </c>
-      <c r="C66" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" t="s">
-        <v>70</v>
-      </c>
-      <c r="D68" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Braavosi culture chain finished, Boashi & Bearded Priest holy orders added
</commit_message>
<xml_diff>
--- a/tsf4's Nightfort/cultural buildings checklist.xlsx
+++ b/tsf4's Nightfort/cultural buildings checklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Culture</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Total troops for each level should = 100, with the overall total at 1000.</t>
-  </si>
-  <si>
     <t>Tax and fort shouldn't be too crazy</t>
   </si>
   <si>
@@ -67,6 +64,15 @@
   </si>
   <si>
     <t>Can always be balanced later, but this should explain my plan.</t>
+  </si>
+  <si>
+    <t>Total troops for each level should be around 100, with overall being around 1000.</t>
+  </si>
+  <si>
+    <t>Troop totals convert into a tenth of their "total" *50 becomes 5, 165 becomes 16.5 rounded to 15, etc)</t>
+  </si>
+  <si>
+    <t>Braavosi City</t>
   </si>
 </sst>
 </file>
@@ -393,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -448,71 +454,420 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2">
+        <v>-0.36</v>
+      </c>
+      <c r="C2">
+        <v>-0.7</v>
+      </c>
+      <c r="H2">
+        <v>35</v>
+      </c>
+      <c r="I2">
+        <v>65</v>
+      </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>-0.05</v>
+      </c>
+      <c r="C3">
+        <v>-0.7</v>
+      </c>
+      <c r="E3">
+        <v>85</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>0.21</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>70</v>
+      </c>
+      <c r="I4">
+        <v>30</v>
+      </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>-0.02</v>
+      </c>
+      <c r="C5">
+        <v>-0.9</v>
+      </c>
+      <c r="F5">
+        <v>80</v>
+      </c>
+      <c r="I5">
+        <v>20</v>
+      </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>-0.25</v>
+      </c>
+      <c r="C6">
+        <v>0.7</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>-0.38</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>0.04</v>
+      </c>
+      <c r="C8">
+        <v>-0.8</v>
+      </c>
+      <c r="E8">
+        <v>60</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>0.22</v>
+      </c>
+      <c r="C9">
+        <v>0.1</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>0.26</v>
+      </c>
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+      <c r="G10">
+        <v>40</v>
+      </c>
+      <c r="H10">
+        <v>40</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>0.08</v>
+      </c>
+      <c r="C11">
+        <v>0.9</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>55</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <f>B2+B3+B4+B5+B6+B7+B8+B9+B10+B11</f>
+        <f>SUM(B2:B11)</f>
+        <v>-0.24999999999999994</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C2:C11)</f>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>145</v>
+      </c>
+      <c r="F12">
+        <v>230</v>
+      </c>
+      <c r="G12">
+        <v>165</v>
+      </c>
+      <c r="H12">
+        <v>145</v>
+      </c>
+      <c r="I12">
+        <v>255</v>
+      </c>
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C13">
+        <v>-0.4</v>
+      </c>
+      <c r="D13">
+        <v>85</v>
+      </c>
+      <c r="H13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>-0.48</v>
+      </c>
+      <c r="C14">
+        <v>0.8</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>0.41</v>
+      </c>
+      <c r="C15">
+        <v>0.8</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="F15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
         <v>0</v>
+      </c>
+      <c r="C16">
+        <v>-0.3</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>0.19</v>
+      </c>
+      <c r="C17">
+        <v>-0.5</v>
+      </c>
+      <c r="G17">
+        <v>55</v>
+      </c>
+      <c r="I17">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>0.19</v>
+      </c>
+      <c r="C18">
+        <v>-0.9</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>0.44</v>
+      </c>
+      <c r="C19">
+        <v>0.8</v>
+      </c>
+      <c r="D19">
+        <v>40</v>
+      </c>
+      <c r="H19">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>0.1</v>
+      </c>
+      <c r="C20">
+        <v>0.9</v>
+      </c>
+      <c r="G20">
+        <v>50</v>
+      </c>
+      <c r="H20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>0.03</v>
+      </c>
+      <c r="C21">
+        <v>-0.8</v>
+      </c>
+      <c r="D21">
+        <v>70</v>
+      </c>
+      <c r="F21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>-0.38</v>
+      </c>
+      <c r="C22">
+        <v>0.1</v>
+      </c>
+      <c r="F22">
+        <v>25</v>
+      </c>
+      <c r="I22">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B13:B22)</f>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="C23">
+        <f>SUM(C13:C22)</f>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="D23">
+        <v>255</v>
+      </c>
+      <c r="E23">
+        <v>185</v>
+      </c>
+      <c r="F23">
+        <v>130</v>
+      </c>
+      <c r="G23">
+        <v>135</v>
+      </c>
+      <c r="H23">
+        <v>125</v>
+      </c>
+      <c r="I23">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
riverland char validator work
</commit_message>
<xml_diff>
--- a/tsf4's Nightfort/cultural buildings checklist.xlsx
+++ b/tsf4's Nightfort/cultural buildings checklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Culture</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Braavosi City</t>
+  </si>
+  <si>
+    <t>Lorathi Castle</t>
   </si>
 </sst>
 </file>
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -870,6 +873,61 @@
         <v>170</v>
       </c>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="597" r:id="rId1"/>

</xml_diff>

<commit_message>
Lorathi castle chain added
</commit_message>
<xml_diff>
--- a/tsf4's Nightfort/cultural buildings checklist.xlsx
+++ b/tsf4's Nightfort/cultural buildings checklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Culture</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Lorathi Castle</t>
+  </si>
+  <si>
+    <t>Tax and fort are halved from total.</t>
+  </si>
+  <si>
+    <t>Lorathi City</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -549,6 +555,9 @@
       <c r="G6">
         <v>70</v>
       </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -1081,6 +1090,138 @@
       </c>
       <c r="I34">
         <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>0.45</v>
+      </c>
+      <c r="C35">
+        <v>-0.2</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>15</v>
+      </c>
+      <c r="I35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36">
+        <v>-0.43</v>
+      </c>
+      <c r="C36">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>-0.43</v>
+      </c>
+      <c r="C37">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>0.18</v>
+      </c>
+      <c r="C38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>0.09</v>
+      </c>
+      <c r="C39">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C41">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>-0.03</v>
+      </c>
+      <c r="C42">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>-0.37</v>
+      </c>
+      <c r="C43">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>-0.08</v>
+      </c>
+      <c r="C44">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <f>SUM(B35:B44)</f>
+        <v>-0.33</v>
+      </c>
+      <c r="C45">
+        <f>SUM(C35:C44)</f>
+        <v>-0.70000000000000018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>